<commit_message>
feat: criar ieds especificos
</commit_message>
<xml_diff>
--- a/lista_arquivos.xlsx
+++ b/lista_arquivos.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="34">
   <si>
     <t>arquivos</t>
   </si>
@@ -40,56 +40,95 @@
     <t>SE</t>
   </si>
   <si>
-    <t>LAB</t>
-  </si>
-  <si>
-    <t>21Y2</t>
-  </si>
-  <si>
-    <t>21Y3</t>
-  </si>
-  <si>
-    <t>11T1</t>
-  </si>
-  <si>
-    <t>11H1</t>
-  </si>
-  <si>
-    <t>12T1</t>
-  </si>
-  <si>
-    <t>12F2</t>
-  </si>
-  <si>
-    <t>12F3</t>
-  </si>
-  <si>
-    <t>10.82.115.104</t>
-  </si>
-  <si>
-    <t>10.82.115.105</t>
-  </si>
-  <si>
-    <t>10.82.115.106</t>
-  </si>
-  <si>
-    <t>10.82.115.107</t>
-  </si>
-  <si>
-    <t>10.82.115.108</t>
-  </si>
-  <si>
-    <t>10.82.115.109</t>
-  </si>
-  <si>
-    <t>10.82.115.110</t>
+    <t>ied</t>
+  </si>
+  <si>
+    <t>IED751</t>
+  </si>
+  <si>
+    <t>IED351A</t>
+  </si>
+  <si>
+    <t>CXS</t>
+  </si>
+  <si>
+    <t>29L1</t>
+  </si>
+  <si>
+    <t>12V4</t>
+  </si>
+  <si>
+    <t>29B1</t>
+  </si>
+  <si>
+    <t>21C6</t>
+  </si>
+  <si>
+    <t>12T3</t>
+  </si>
+  <si>
+    <t>11B3</t>
+  </si>
+  <si>
+    <t>21C7</t>
+  </si>
+  <si>
+    <t>29L2</t>
+  </si>
+  <si>
+    <t>29L3</t>
+  </si>
+  <si>
+    <t>21C8</t>
+  </si>
+  <si>
+    <t>29L4</t>
+  </si>
+  <si>
+    <t>11C9</t>
+  </si>
+  <si>
+    <t>10.10.34.165</t>
+  </si>
+  <si>
+    <t>10.10.34.168</t>
+  </si>
+  <si>
+    <t>10.10.34.173</t>
+  </si>
+  <si>
+    <t>10.10.34.174</t>
+  </si>
+  <si>
+    <t>10.10.34.175</t>
+  </si>
+  <si>
+    <t>10.10.34.178</t>
+  </si>
+  <si>
+    <t>10.10.34.179</t>
+  </si>
+  <si>
+    <t>10.10.34.180</t>
+  </si>
+  <si>
+    <t>10.10.34.183</t>
+  </si>
+  <si>
+    <t>10.10.34.186</t>
+  </si>
+  <si>
+    <t>10.10.34.187</t>
+  </si>
+  <si>
+    <t>10.10.34.102</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -125,6 +164,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -152,7 +199,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -172,6 +219,10 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -463,239 +514,361 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F17"/>
+  <dimension ref="A1:G17"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.85546875" style="1" customWidth="1"/>
-    <col min="5" max="5" width="27.5703125" style="1" customWidth="1"/>
-    <col min="6" max="6" width="29.7109375" style="1" customWidth="1"/>
+    <col min="3" max="3" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.85546875" style="1" customWidth="1"/>
+    <col min="6" max="6" width="27.5703125" style="1" customWidth="1"/>
+    <col min="7" max="7" width="29.7109375" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="C1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B2" s="6" t="s">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" s="4" t="str">
+        <f>CONCATENATE(B2,C2)</f>
+        <v>CXS29L1</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="F2" s="4" t="str">
+        <f t="shared" ref="F2" si="0">CONCATENATE(D2,"_CMD_SEL.xml")</f>
+        <v>CXS29L1_CMD_SEL.xml</v>
+      </c>
+      <c r="G2" s="4" t="str">
+        <f t="shared" ref="G2" si="1">CONCATENATE(D2,"_COMANDOS.xml")</f>
+        <v>CXS29L1_COMANDOS.xml</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" s="4" t="str">
+        <f t="shared" ref="D3:D13" si="2">CONCATENATE(B3,C3)</f>
+        <v>CXS12V4</v>
+      </c>
+      <c r="E3" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="F3" s="4" t="str">
+        <f t="shared" ref="F3" si="3">CONCATENATE(D3,"_CMD_SEL.xml")</f>
+        <v>CXS12V4_CMD_SEL.xml</v>
+      </c>
+      <c r="G3" s="4" t="str">
+        <f t="shared" ref="G3" si="4">CONCATENATE(D3,"_COMANDOS.xml")</f>
+        <v>CXS12V4_COMANDOS.xml</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="D4" s="4" t="str">
+        <f t="shared" si="2"/>
+        <v>CXS29B1</v>
+      </c>
+      <c r="E4" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="F4" s="4" t="str">
+        <f t="shared" ref="F4:F8" si="5">CONCATENATE(D4,"_CMD_SEL.xml")</f>
+        <v>CXS29B1_CMD_SEL.xml</v>
+      </c>
+      <c r="G4" s="4" t="str">
+        <f t="shared" ref="G4:G8" si="6">CONCATENATE(D4,"_COMANDOS.xml")</f>
+        <v>CXS29B1_COMANDOS.xml</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="D5" s="4" t="str">
+        <f t="shared" si="2"/>
+        <v>CXS21C6</v>
+      </c>
+      <c r="E5" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="F5" s="4" t="str">
+        <f t="shared" si="5"/>
+        <v>CXS21C6_CMD_SEL.xml</v>
+      </c>
+      <c r="G5" s="4" t="str">
+        <f t="shared" si="6"/>
+        <v>CXS21C6_COMANDOS.xml</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="D6" s="4" t="str">
+        <f t="shared" si="2"/>
+        <v>CXS12T3</v>
+      </c>
+      <c r="E6" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="F6" s="4" t="str">
+        <f t="shared" si="5"/>
+        <v>CXS12T3_CMD_SEL.xml</v>
+      </c>
+      <c r="G6" s="4" t="str">
+        <f t="shared" si="6"/>
+        <v>CXS12T3_COMANDOS.xml</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="D7" s="4" t="str">
+        <f t="shared" si="2"/>
+        <v>CXS11B3</v>
+      </c>
+      <c r="E7" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="F7" s="4" t="str">
+        <f t="shared" si="5"/>
+        <v>CXS11B3_CMD_SEL.xml</v>
+      </c>
+      <c r="G7" s="4" t="str">
+        <f t="shared" si="6"/>
+        <v>CXS11B3_COMANDOS.xml</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C8" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="D8" s="4" t="str">
+        <f t="shared" si="2"/>
+        <v>CXS21C7</v>
+      </c>
+      <c r="E8" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="F8" s="4" t="str">
+        <f t="shared" si="5"/>
+        <v>CXS21C7_CMD_SEL.xml</v>
+      </c>
+      <c r="G8" s="4" t="str">
+        <f t="shared" si="6"/>
+        <v>CXS21C7_COMANDOS.xml</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="D9" s="4" t="str">
+        <f t="shared" si="2"/>
+        <v>CXS29L2</v>
+      </c>
+      <c r="E9" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="F9" s="4" t="str">
+        <f t="shared" ref="F9:F13" si="7">CONCATENATE(D9,"_CMD_SEL.xml")</f>
+        <v>CXS29L2_CMD_SEL.xml</v>
+      </c>
+      <c r="G9" s="4" t="str">
+        <f t="shared" ref="G9:G13" si="8">CONCATENATE(D9,"_COMANDOS.xml")</f>
+        <v>CXS29L2_COMANDOS.xml</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="D10" s="4" t="str">
+        <f t="shared" si="2"/>
+        <v>CXS29L3</v>
+      </c>
+      <c r="E10" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="F10" s="4" t="str">
+        <f t="shared" si="7"/>
+        <v>CXS29L3_CMD_SEL.xml</v>
+      </c>
+      <c r="G10" s="4" t="str">
+        <f t="shared" si="8"/>
+        <v>CXS29L3_COMANDOS.xml</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="D11" s="4" t="str">
+        <f t="shared" si="2"/>
+        <v>CXS21C8</v>
+      </c>
+      <c r="E11" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="F11" s="4" t="str">
+        <f t="shared" si="7"/>
+        <v>CXS21C8_CMD_SEL.xml</v>
+      </c>
+      <c r="G11" s="4" t="str">
+        <f t="shared" si="8"/>
+        <v>CXS21C8_COMANDOS.xml</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="D12" s="4" t="str">
+        <f t="shared" si="2"/>
+        <v>CXS29L4</v>
+      </c>
+      <c r="E12" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="F12" s="4" t="str">
+        <f t="shared" si="7"/>
+        <v>CXS29L4_CMD_SEL.xml</v>
+      </c>
+      <c r="G12" s="4" t="str">
+        <f t="shared" si="8"/>
+        <v>CXS29L4_COMANDOS.xml</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="4" t="str">
-        <f>CONCATENATE(A2,"_",B2)</f>
-        <v>LAB_21Y2</v>
-      </c>
-      <c r="D2" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="E2" s="4" t="str">
-        <f t="shared" ref="E2" si="0">CONCATENATE(C2,"_CMD_SEL.xml")</f>
-        <v>LAB_21Y2_CMD_SEL.xml</v>
-      </c>
-      <c r="F2" s="4" t="str">
-        <f t="shared" ref="F2" si="1">CONCATENATE(C2,"_COMANDOS.xml")</f>
-        <v>LAB_21Y2_COMANDOS.xml</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="C3" s="4" t="str">
-        <f t="shared" ref="C3:C8" si="2">CONCATENATE(A3,"_",B3)</f>
-        <v>LAB_21Y3</v>
-      </c>
-      <c r="D3" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="E3" s="4" t="str">
-        <f t="shared" ref="E3" si="3">CONCATENATE(C3,"_CMD_SEL.xml")</f>
-        <v>LAB_21Y3_CMD_SEL.xml</v>
-      </c>
-      <c r="F3" s="4" t="str">
-        <f t="shared" ref="F3" si="4">CONCATENATE(C3,"_COMANDOS.xml")</f>
-        <v>LAB_21Y3_COMANDOS.xml</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="C4" s="4" t="str">
-        <f t="shared" si="2"/>
-        <v>LAB_11T1</v>
-      </c>
-      <c r="D4" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="E4" s="4" t="str">
-        <f t="shared" ref="E4:E8" si="5">CONCATENATE(C4,"_CMD_SEL.xml")</f>
-        <v>LAB_11T1_CMD_SEL.xml</v>
-      </c>
-      <c r="F4" s="4" t="str">
-        <f t="shared" ref="F4:F8" si="6">CONCATENATE(C4,"_COMANDOS.xml")</f>
-        <v>LAB_11T1_COMANDOS.xml</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B5" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="C5" s="4" t="str">
-        <f t="shared" si="2"/>
-        <v>LAB_11H1</v>
-      </c>
-      <c r="D5" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="E5" s="4" t="str">
-        <f t="shared" si="5"/>
-        <v>LAB_11H1_CMD_SEL.xml</v>
-      </c>
-      <c r="F5" s="4" t="str">
-        <f t="shared" si="6"/>
-        <v>LAB_11H1_COMANDOS.xml</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B6" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="C6" s="4" t="str">
-        <f t="shared" si="2"/>
-        <v>LAB_12T1</v>
-      </c>
-      <c r="D6" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="E6" s="4" t="str">
-        <f t="shared" si="5"/>
-        <v>LAB_12T1_CMD_SEL.xml</v>
-      </c>
-      <c r="F6" s="4" t="str">
-        <f t="shared" si="6"/>
-        <v>LAB_12T1_COMANDOS.xml</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B7" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="C7" s="4" t="str">
-        <f t="shared" si="2"/>
-        <v>LAB_12F2</v>
-      </c>
-      <c r="D7" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="E7" s="4" t="str">
-        <f t="shared" si="5"/>
-        <v>LAB_12F2_CMD_SEL.xml</v>
-      </c>
-      <c r="F7" s="4" t="str">
-        <f t="shared" si="6"/>
-        <v>LAB_12F2_COMANDOS.xml</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B8" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="C8" s="4" t="str">
-        <f t="shared" si="2"/>
-        <v>LAB_12F3</v>
-      </c>
-      <c r="D8" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="E8" s="4" t="str">
-        <f t="shared" si="5"/>
-        <v>LAB_12F3_CMD_SEL.xml</v>
-      </c>
-      <c r="F8" s="4" t="str">
-        <f t="shared" si="6"/>
-        <v>LAB_12F3_COMANDOS.xml</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="3"/>
-      <c r="B9" s="6"/>
-      <c r="C9" s="4"/>
-      <c r="D9" s="6"/>
-      <c r="E9" s="4"/>
-      <c r="F9" s="4"/>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="3"/>
-      <c r="B10" s="5"/>
-      <c r="C10" s="4"/>
-      <c r="D10" s="5"/>
-      <c r="E10" s="4"/>
-      <c r="F10" s="4"/>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="3"/>
-      <c r="B11" s="5"/>
-      <c r="C11" s="4"/>
-      <c r="D11" s="5"/>
-      <c r="E11" s="4"/>
-      <c r="F11" s="4"/>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="3"/>
-      <c r="B12" s="5"/>
-      <c r="C12" s="4"/>
-      <c r="D12" s="5"/>
-      <c r="E12" s="4"/>
-      <c r="F12" s="4"/>
-    </row>
-    <row r="17" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C17"/>
+      <c r="B13" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D13" s="4" t="str">
+        <f t="shared" si="2"/>
+        <v>CXS11C9</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="F13" s="4" t="str">
+        <f t="shared" si="7"/>
+        <v>CXS11C9_CMD_SEL.xml</v>
+      </c>
+      <c r="G13" s="4" t="str">
+        <f t="shared" si="8"/>
+        <v>CXS11C9_COMANDOS.xml</v>
+      </c>
+    </row>
+    <row r="17" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D17"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="D12:D1048576 D1">
+  <conditionalFormatting sqref="E12:E1048576 E1">
     <cfRule type="duplicateValues" dxfId="0" priority="2"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>